<commit_message>
Solving github issue #74: improving util_funtions.identity_rcot() to handle the case where set labels for rows and columns are ordered differently with respect to the variable.related_dims_map dataframe. Tests expanded and modified accordingly. Set file of the feature/constant test case modified to reflect this case.
</commit_message>
<xml_diff>
--- a/tests/models/features/constants/sets.xlsx
+++ b/tests/models/features/constants/sets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\integration\units\constants\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\models\features\constants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC19F4F-F454-4CCD-A85B-956EE3D3782D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FEAB19-F6E1-4CFA-B71D-BABD6DA8426D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32140" yWindow="2990" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6630" yWindow="2630" windowWidth="18840" windowHeight="15800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_set_FLOWS" sheetId="2" r:id="rId1"/>
@@ -428,14 +428,12 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -514,7 +512,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -533,7 +531,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -541,18 +539,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>